<commit_message>
Remove machine key as input from user
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Machines.xlsx
+++ b/Workbooks/EN/Machines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A03B4F-39E4-49F8-887D-B8AB915901A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A20D8EC-4BEE-4836-A5B5-69AC950FE7D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -272,15 +272,79 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -400,53 +464,6 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="5"/>
@@ -469,70 +486,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="5"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="5"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
@@ -647,10 +600,21 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -676,6 +640,37 @@
           <bgColor theme="2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -691,13 +686,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:D201" headerRowDxfId="9" dataDxfId="16" totalsRowDxfId="8" headerRowBorderDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:D201" headerRowDxfId="16" dataDxfId="14" totalsRowDxfId="12" headerRowBorderDxfId="15" tableBorderDxfId="13">
   <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Type" totalsRowLabel="Total" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Key" totalsRowFunction="count" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Type" totalsRowLabel="Total" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Key" totalsRowFunction="count" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,10 +703,10 @@
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4D652F4A-5125-4BA7-BCE0-BCD13A330E29}" name="Key" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4D652F4A-5125-4BA7-BCE0-BCD13A330E29}" name="Key" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -721,9 +716,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C201" totalsRowShown="0">
   <autoFilter ref="A1:C201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2258,1416 +2253,1416 @@
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="19"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="19"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="19"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="19"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="19"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="19"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="19"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="19"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="19"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="19"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="19"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="19"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="19"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="19"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="19"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="19"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="17"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="19"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="17"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="19"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="19"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="17"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="19"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="17"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="19"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="17"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="19"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="17"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="17"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="19"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="17"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="19"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="17"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="19"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="17"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="17"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="19"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="17"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="19"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="17"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="19"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="17"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="19"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="17"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="19"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="7"/>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="17"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="19"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="7"/>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="17"/>
-      <c r="B94" s="17"/>
-      <c r="C94" s="19"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="17"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="19"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="17"/>
-      <c r="B96" s="17"/>
-      <c r="C96" s="19"/>
+      <c r="B96" s="19"/>
+      <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="17"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="19"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="19"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="17"/>
-      <c r="B99" s="17"/>
-      <c r="C99" s="19"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="7"/>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="19"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="17"/>
-      <c r="B101" s="17"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="17"/>
-      <c r="B102" s="17"/>
-      <c r="C102" s="19"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="17"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="19"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="17"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="19"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="17"/>
-      <c r="B105" s="17"/>
-      <c r="C105" s="19"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
-      <c r="C106" s="19"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="17"/>
-      <c r="B107" s="17"/>
-      <c r="C107" s="19"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="17"/>
-      <c r="B108" s="17"/>
-      <c r="C108" s="19"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="17"/>
-      <c r="B109" s="17"/>
-      <c r="C109" s="19"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="17"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="19"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="17"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="19"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="17"/>
-      <c r="B112" s="17"/>
-      <c r="C112" s="19"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="17"/>
-      <c r="B113" s="17"/>
-      <c r="C113" s="19"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="17"/>
-      <c r="B114" s="17"/>
-      <c r="C114" s="19"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="19"/>
+      <c r="B115" s="19"/>
+      <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="17"/>
-      <c r="B116" s="17"/>
-      <c r="C116" s="19"/>
+      <c r="B116" s="19"/>
+      <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="19"/>
+      <c r="B117" s="19"/>
+      <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="17"/>
-      <c r="B118" s="17"/>
-      <c r="C118" s="19"/>
+      <c r="B118" s="19"/>
+      <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="17"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="19"/>
+      <c r="B119" s="19"/>
+      <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="17"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="19"/>
+      <c r="B120" s="19"/>
+      <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="7"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="19"/>
+      <c r="B121" s="19"/>
+      <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="19"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="19"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="7"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="17"/>
-      <c r="B124" s="17"/>
-      <c r="C124" s="19"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="17"/>
-      <c r="B125" s="17"/>
-      <c r="C125" s="19"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="17"/>
-      <c r="B126" s="17"/>
-      <c r="C126" s="19"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="17"/>
-      <c r="B127" s="17"/>
-      <c r="C127" s="19"/>
+      <c r="B127" s="19"/>
+      <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="17"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="19"/>
+      <c r="B128" s="19"/>
+      <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="17"/>
-      <c r="B129" s="17"/>
-      <c r="C129" s="19"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="7"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="17"/>
-      <c r="B130" s="17"/>
-      <c r="C130" s="19"/>
+      <c r="B130" s="19"/>
+      <c r="C130" s="7"/>
       <c r="D130" s="7"/>
       <c r="E130" s="7"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="17"/>
-      <c r="B131" s="17"/>
-      <c r="C131" s="19"/>
+      <c r="B131" s="19"/>
+      <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="17"/>
-      <c r="B132" s="17"/>
-      <c r="C132" s="19"/>
+      <c r="B132" s="19"/>
+      <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="17"/>
-      <c r="B133" s="17"/>
-      <c r="C133" s="19"/>
+      <c r="B133" s="19"/>
+      <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="17"/>
-      <c r="B134" s="17"/>
-      <c r="C134" s="19"/>
+      <c r="B134" s="19"/>
+      <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="17"/>
-      <c r="B135" s="17"/>
-      <c r="C135" s="19"/>
+      <c r="B135" s="19"/>
+      <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="17"/>
-      <c r="B136" s="17"/>
-      <c r="C136" s="19"/>
+      <c r="B136" s="19"/>
+      <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="17"/>
-      <c r="B137" s="17"/>
-      <c r="C137" s="19"/>
+      <c r="B137" s="19"/>
+      <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="7"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="17"/>
-      <c r="B138" s="17"/>
-      <c r="C138" s="19"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="17"/>
-      <c r="B139" s="17"/>
-      <c r="C139" s="19"/>
+      <c r="B139" s="19"/>
+      <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="17"/>
-      <c r="B140" s="17"/>
-      <c r="C140" s="19"/>
+      <c r="B140" s="19"/>
+      <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="7"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="17"/>
-      <c r="B141" s="17"/>
-      <c r="C141" s="19"/>
+      <c r="B141" s="19"/>
+      <c r="C141" s="7"/>
       <c r="D141" s="7"/>
       <c r="E141" s="7"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="17"/>
-      <c r="B142" s="17"/>
-      <c r="C142" s="19"/>
+      <c r="B142" s="19"/>
+      <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="7"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="17"/>
-      <c r="B143" s="17"/>
-      <c r="C143" s="19"/>
+      <c r="B143" s="19"/>
+      <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="17"/>
-      <c r="B144" s="17"/>
-      <c r="C144" s="19"/>
+      <c r="B144" s="19"/>
+      <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="7"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="17"/>
-      <c r="B145" s="17"/>
-      <c r="C145" s="19"/>
+      <c r="B145" s="19"/>
+      <c r="C145" s="7"/>
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="17"/>
-      <c r="B146" s="17"/>
-      <c r="C146" s="19"/>
+      <c r="B146" s="19"/>
+      <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="17"/>
-      <c r="B147" s="17"/>
-      <c r="C147" s="19"/>
+      <c r="B147" s="19"/>
+      <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="17"/>
-      <c r="B148" s="17"/>
-      <c r="C148" s="19"/>
+      <c r="B148" s="19"/>
+      <c r="C148" s="7"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="17"/>
-      <c r="B149" s="17"/>
-      <c r="C149" s="19"/>
+      <c r="B149" s="19"/>
+      <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="17"/>
-      <c r="B150" s="17"/>
-      <c r="C150" s="19"/>
+      <c r="B150" s="19"/>
+      <c r="C150" s="7"/>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="17"/>
-      <c r="B151" s="17"/>
-      <c r="C151" s="19"/>
+      <c r="B151" s="19"/>
+      <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="17"/>
-      <c r="B152" s="17"/>
-      <c r="C152" s="19"/>
+      <c r="B152" s="19"/>
+      <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="17"/>
-      <c r="B153" s="17"/>
-      <c r="C153" s="19"/>
+      <c r="B153" s="19"/>
+      <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="17"/>
-      <c r="B154" s="17"/>
-      <c r="C154" s="19"/>
+      <c r="B154" s="19"/>
+      <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="17"/>
-      <c r="B155" s="17"/>
-      <c r="C155" s="19"/>
+      <c r="B155" s="19"/>
+      <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="17"/>
-      <c r="B156" s="17"/>
-      <c r="C156" s="19"/>
+      <c r="B156" s="19"/>
+      <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="17"/>
-      <c r="B157" s="17"/>
-      <c r="C157" s="19"/>
+      <c r="B157" s="19"/>
+      <c r="C157" s="7"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="17"/>
-      <c r="B158" s="17"/>
-      <c r="C158" s="19"/>
+      <c r="B158" s="19"/>
+      <c r="C158" s="7"/>
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="17"/>
-      <c r="B159" s="17"/>
-      <c r="C159" s="19"/>
+      <c r="B159" s="19"/>
+      <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="17"/>
-      <c r="B160" s="17"/>
-      <c r="C160" s="19"/>
+      <c r="B160" s="19"/>
+      <c r="C160" s="7"/>
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="17"/>
-      <c r="B161" s="17"/>
-      <c r="C161" s="19"/>
+      <c r="B161" s="19"/>
+      <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="17"/>
-      <c r="B162" s="17"/>
-      <c r="C162" s="19"/>
+      <c r="B162" s="19"/>
+      <c r="C162" s="7"/>
       <c r="D162" s="7"/>
       <c r="E162" s="7"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="17"/>
-      <c r="B163" s="17"/>
-      <c r="C163" s="19"/>
+      <c r="B163" s="19"/>
+      <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="17"/>
-      <c r="B164" s="17"/>
-      <c r="C164" s="19"/>
+      <c r="B164" s="19"/>
+      <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="17"/>
-      <c r="B165" s="17"/>
-      <c r="C165" s="19"/>
+      <c r="B165" s="19"/>
+      <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="17"/>
-      <c r="B166" s="17"/>
-      <c r="C166" s="19"/>
+      <c r="B166" s="19"/>
+      <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="17"/>
-      <c r="B167" s="17"/>
-      <c r="C167" s="19"/>
+      <c r="B167" s="19"/>
+      <c r="C167" s="7"/>
       <c r="D167" s="7"/>
       <c r="E167" s="7"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="17"/>
-      <c r="B168" s="17"/>
-      <c r="C168" s="19"/>
+      <c r="B168" s="19"/>
+      <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="7"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="17"/>
-      <c r="B169" s="17"/>
-      <c r="C169" s="19"/>
+      <c r="B169" s="19"/>
+      <c r="C169" s="7"/>
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="17"/>
-      <c r="B170" s="17"/>
-      <c r="C170" s="19"/>
+      <c r="B170" s="19"/>
+      <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="17"/>
-      <c r="B171" s="17"/>
-      <c r="C171" s="19"/>
+      <c r="B171" s="19"/>
+      <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="7"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="17"/>
-      <c r="B172" s="17"/>
-      <c r="C172" s="19"/>
+      <c r="B172" s="19"/>
+      <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="17"/>
-      <c r="B173" s="17"/>
-      <c r="C173" s="19"/>
+      <c r="B173" s="19"/>
+      <c r="C173" s="7"/>
       <c r="D173" s="7"/>
       <c r="E173" s="7"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="17"/>
-      <c r="B174" s="17"/>
-      <c r="C174" s="19"/>
+      <c r="B174" s="19"/>
+      <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="17"/>
-      <c r="B175" s="17"/>
-      <c r="C175" s="19"/>
+      <c r="B175" s="19"/>
+      <c r="C175" s="7"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="17"/>
-      <c r="B176" s="17"/>
-      <c r="C176" s="19"/>
+      <c r="B176" s="19"/>
+      <c r="C176" s="7"/>
       <c r="D176" s="7"/>
       <c r="E176" s="7"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="17"/>
-      <c r="B177" s="17"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="7"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="17"/>
-      <c r="B178" s="17"/>
-      <c r="C178" s="19"/>
+      <c r="B178" s="19"/>
+      <c r="C178" s="7"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="17"/>
-      <c r="B179" s="17"/>
-      <c r="C179" s="19"/>
+      <c r="B179" s="19"/>
+      <c r="C179" s="7"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="17"/>
-      <c r="B180" s="17"/>
-      <c r="C180" s="19"/>
+      <c r="B180" s="19"/>
+      <c r="C180" s="7"/>
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="17"/>
-      <c r="B181" s="17"/>
-      <c r="C181" s="19"/>
+      <c r="B181" s="19"/>
+      <c r="C181" s="7"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="17"/>
-      <c r="B182" s="17"/>
-      <c r="C182" s="19"/>
+      <c r="B182" s="19"/>
+      <c r="C182" s="7"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="17"/>
-      <c r="B183" s="17"/>
-      <c r="C183" s="19"/>
+      <c r="B183" s="19"/>
+      <c r="C183" s="7"/>
       <c r="D183" s="7"/>
       <c r="E183" s="7"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="17"/>
-      <c r="B184" s="17"/>
-      <c r="C184" s="19"/>
+      <c r="B184" s="19"/>
+      <c r="C184" s="7"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="17"/>
-      <c r="B185" s="17"/>
-      <c r="C185" s="19"/>
+      <c r="B185" s="19"/>
+      <c r="C185" s="7"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="17"/>
-      <c r="B186" s="17"/>
-      <c r="C186" s="19"/>
+      <c r="B186" s="19"/>
+      <c r="C186" s="7"/>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="17"/>
-      <c r="B187" s="17"/>
-      <c r="C187" s="19"/>
+      <c r="B187" s="19"/>
+      <c r="C187" s="7"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="17"/>
-      <c r="B188" s="17"/>
-      <c r="C188" s="19"/>
+      <c r="B188" s="19"/>
+      <c r="C188" s="7"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="17"/>
-      <c r="B189" s="17"/>
-      <c r="C189" s="19"/>
+      <c r="B189" s="19"/>
+      <c r="C189" s="7"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="17"/>
-      <c r="B190" s="17"/>
-      <c r="C190" s="19"/>
+      <c r="B190" s="19"/>
+      <c r="C190" s="7"/>
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="17"/>
-      <c r="B191" s="17"/>
-      <c r="C191" s="19"/>
+      <c r="B191" s="19"/>
+      <c r="C191" s="7"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="17"/>
-      <c r="B192" s="17"/>
-      <c r="C192" s="19"/>
+      <c r="B192" s="19"/>
+      <c r="C192" s="7"/>
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="17"/>
-      <c r="B193" s="17"/>
-      <c r="C193" s="19"/>
+      <c r="B193" s="19"/>
+      <c r="C193" s="7"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="17"/>
-      <c r="B194" s="17"/>
-      <c r="C194" s="19"/>
+      <c r="B194" s="19"/>
+      <c r="C194" s="7"/>
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="17"/>
-      <c r="B195" s="17"/>
-      <c r="C195" s="19"/>
+      <c r="B195" s="19"/>
+      <c r="C195" s="7"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="17"/>
-      <c r="B196" s="17"/>
-      <c r="C196" s="19"/>
+      <c r="B196" s="19"/>
+      <c r="C196" s="7"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="17"/>
-      <c r="B197" s="17"/>
-      <c r="C197" s="19"/>
+      <c r="B197" s="19"/>
+      <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="17"/>
-      <c r="B198" s="17"/>
-      <c r="C198" s="19"/>
+      <c r="B198" s="19"/>
+      <c r="C198" s="7"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="17"/>
-      <c r="B199" s="17"/>
-      <c r="C199" s="19"/>
+      <c r="B199" s="19"/>
+      <c r="C199" s="7"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="17"/>
-      <c r="B200" s="17"/>
-      <c r="C200" s="19"/>
+      <c r="B200" s="19"/>
+      <c r="C200" s="7"/>
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="17"/>
-      <c r="B201" s="17"/>
-      <c r="C201" s="19"/>
+      <c r="B201" s="19"/>
+      <c r="C201" s="7"/>
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
     </row>
@@ -3711,7 +3706,7 @@
       <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve formatting of workbooks
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Machines.xlsx
+++ b/Workbooks/EN/Machines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABC86BE-A84A-46B6-9643-624EADEA6581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0563DB3-70BF-4689-96DB-A767D1273C53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -308,31 +308,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
@@ -393,6 +368,31 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -702,7 +702,7 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{4D652F4A-5125-4BA7-BCE0-BCD13A330E29}" name="Key" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,8 +712,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C201" totalsRowShown="0">
   <autoFilter ref="A1:C201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Name" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -991,10 +991,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="1" max="2" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2240,12 +2239,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.7265625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3696,9 +3695,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="43.54296875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="3" width="45.7265625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>